<commit_message>
MVP - all routes and views work
</commit_message>
<xml_diff>
--- a/setup_files/Gifts App Restful Routing Chart.xlsx
+++ b/setup_files/Gifts App Restful Routing Chart.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dw00830/Desktop/sei/projects/AndyProject2/setup_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{93FC081B-3B04-C443-8E16-4AD5C234DEF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A1AE30C-D078-FC48-A00C-3F2DC5DBB276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="220" yWindow="500" windowWidth="33600" windowHeight="18680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Gifts_version" sheetId="2" r:id="rId1"/>
+    <sheet name="Template" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="113">
   <si>
     <t>CRUD</t>
   </si>
@@ -262,13 +263,126 @@
   </si>
   <si>
     <t>Delete an existing player</t>
+  </si>
+  <si>
+    <t>GIFT APP - User Resource</t>
+  </si>
+  <si>
+    <t>GIFT APP - Gift Resource</t>
+  </si>
+  <si>
+    <t>Gift app homepage with login/signup links</t>
+  </si>
+  <si>
+    <t>GIFT APP - Giver Resource</t>
+  </si>
+  <si>
+    <t>User.findAll({
+    where: {username: req.body.username,
+      password: req.body.password}  } )</t>
+  </si>
+  <si>
+    <t>/users/:id/tasks</t>
+  </si>
+  <si>
+    <t>users/tasks.ejs</t>
+  </si>
+  <si>
+    <t>Tasks</t>
+  </si>
+  <si>
+    <t>Show common Tasks that a User may want to perfrom</t>
+  </si>
+  <si>
+    <t>/users/:id/list</t>
+  </si>
+  <si>
+    <t>User.findByPk(req.params.id, {
+        include: [{ model: Giver }],
+    })</t>
+  </si>
+  <si>
+    <t>users/list.ejs</t>
+  </si>
+  <si>
+    <t>List all Givers assigned to that User</t>
+  </si>
+  <si>
+    <t>/users/:id/profile</t>
+  </si>
+  <si>
+    <t>/givers</t>
+  </si>
+  <si>
+    <t>Giver.findAll( {
+        include: [{ model: User }],
+    })</t>
+  </si>
+  <si>
+    <t>givers/index.ejs</t>
+  </si>
+  <si>
+    <t>Render all Givers from DB</t>
+  </si>
+  <si>
+    <t>/givers/:id</t>
+  </si>
+  <si>
+    <t>Giver.findByPk(req.params.id, {
+        include: [{ model: User }],
+    })</t>
+  </si>
+  <si>
+    <t>givers/profile.ejs</t>
+  </si>
+  <si>
+    <t>SHOW/UPDATE</t>
+  </si>
+  <si>
+    <t>Render one Giver from DB</t>
+  </si>
+  <si>
+    <t>/givers/new</t>
+  </si>
+  <si>
+    <t>givers/newgiver.ejs</t>
+  </si>
+  <si>
+    <t>Render empty Giver form</t>
+  </si>
+  <si>
+    <t>Giver.create(req.body)</t>
+  </si>
+  <si>
+    <t>Create new instance of a Giver then redirect</t>
+  </si>
+  <si>
+    <t>Giver.update(req.body, {
+        where: {id: req.params.id},
+        returning: true,
+    })</t>
+  </si>
+  <si>
+    <t>Updates an existing Giver</t>
+  </si>
+  <si>
+    <t>/givers:id</t>
+  </si>
+  <si>
+    <t>Deletes a Giver</t>
+  </si>
+  <si>
+    <t>Giver.destroy({
+        where: {id: req.params.id},
+        returning: true,
+    })</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -295,6 +409,17 @@
     </font>
     <font>
       <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -343,7 +468,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -431,11 +556,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -564,6 +704,48 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -779,13 +961,610 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCB516FC-9944-E94B-BF0F-790072257F16}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:G30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="17.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" customWidth="1"/>
+    <col min="4" max="4" width="41.5" customWidth="1"/>
+    <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="6" max="6" width="32" customWidth="1"/>
+    <col min="7" max="7" width="56.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="42"/>
+    </row>
+    <row r="3" spans="1:7" ht="57" x14ac:dyDescent="0.2">
+      <c r="A3" s="54" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="54" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="54" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="55" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="54" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="54" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="57" x14ac:dyDescent="0.2">
+      <c r="A4" s="54" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="54" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="54" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" s="55" t="s">
+        <v>99</v>
+      </c>
+      <c r="E4" s="54" t="s">
+        <v>100</v>
+      </c>
+      <c r="F4" s="54" t="s">
+        <v>101</v>
+      </c>
+      <c r="G4" s="54" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="54" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="54" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="54" t="s">
+        <v>104</v>
+      </c>
+      <c r="F5" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="54" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="54" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="54" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="E6" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="54" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="54" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="76" x14ac:dyDescent="0.2">
+      <c r="A7" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="54" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" s="55" t="s">
+        <v>108</v>
+      </c>
+      <c r="E7" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="54" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="76" x14ac:dyDescent="0.2">
+      <c r="A8" s="54" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="54" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" s="55" t="s">
+        <v>112</v>
+      </c>
+      <c r="E8" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="54" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="10" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="42"/>
+    </row>
+    <row r="11" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="56" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="56" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="56" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="56" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="56" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="56" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="56" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="56" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="56" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="56" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="56" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="56" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="56" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="56" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="56" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="56" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="56" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="56" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="57" t="s">
+        <v>84</v>
+      </c>
+      <c r="E15" s="56" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="56" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" s="56" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="56" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="56" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="57" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="56" t="s">
+        <v>86</v>
+      </c>
+      <c r="F16" s="56" t="s">
+        <v>87</v>
+      </c>
+      <c r="G16" s="58" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="56" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" s="57" t="s">
+        <v>90</v>
+      </c>
+      <c r="E17" s="56" t="s">
+        <v>91</v>
+      </c>
+      <c r="F17" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="58" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="56" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="56" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" s="56" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" s="56" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="56" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="56" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="56" t="s">
+        <v>93</v>
+      </c>
+      <c r="D19" s="58" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="56" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19" s="56" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="56" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="56" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="56" t="s">
+        <v>93</v>
+      </c>
+      <c r="D20" s="58" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" s="56" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="56" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20" s="56" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A22" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" s="41"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="42"/>
+    </row>
+    <row r="23" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A23" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="46"/>
+      <c r="D23" s="46"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="G23" s="47" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A24" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="G24" s="50" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A25" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" s="50" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A26" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="49"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="G26" s="50" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A27" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="49" t="s">
+        <v>29</v>
+      </c>
+      <c r="G27" s="50" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A28" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="G28" s="50" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A29" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="49" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="G29" s="50" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A30" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="52" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="52"/>
+      <c r="D30" s="52"/>
+      <c r="E30" s="52"/>
+      <c r="F30" s="52" t="s">
+        <v>41</v>
+      </c>
+      <c r="G30" s="53" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="A22:G22"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;R_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;KFF0000 Company Use</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>

</xml_diff>